<commit_message>
add done checkbox & adjust layout
</commit_message>
<xml_diff>
--- a/repairDB/Personnel.xlsx
+++ b/repairDB/Personnel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MRT DATA\Repair_TRTC\repairDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4069533D-A741-48E1-ADE4-DE8FB271A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494DB8AF-3867-41E0-A389-9B869559335D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="2700" windowWidth="23040" windowHeight="12120" xr2:uid="{AFEE9620-879D-42AA-95F2-C93E683A73FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>人員</t>
   </si>
@@ -54,6 +54,17 @@
   </si>
   <si>
     <t>黃禮志</t>
+  </si>
+  <si>
+    <t>王柏融</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金智媛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姜諧潾</t>
   </si>
 </sst>
 </file>
@@ -99,10 +110,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -440,42 +448,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4850EE-66D5-40F5-9E9E-0938B4CCE777}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>